<commit_message>
update common and testcase file
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/ServiceCollectionTcs.xlsx
+++ b/src/main/resources/excels/ServiceCollectionTcs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FCEFE4-8187-45F2-AD03-F5EDD7E40297}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C55985-F222-4A3D-8C2C-8696A231C1F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -259,12 +259,56 @@
   <si>
     <t>PASS</t>
   </si>
+  <si>
+    <t>SC16</t>
+  </si>
+  <si>
+    <t>Verify text</t>
+  </si>
+  <si>
+    <t>1. Login to Dashboard
+2. Go to Services &gt;&gt; Create service collection
+3. Verify text</t>
+  </si>
+  <si>
+    <t>All text should be shown correctly</t>
+  </si>
+  <si>
+    <t>SC17</t>
+  </si>
+  <si>
+    <t>Verify automated collection when has new service meets the condition</t>
+  </si>
+  <si>
+    <t>1. Login to Dashboard
+2. Go to 2. Go to Services &gt;&gt; Create service collection (Automated)
+3. Call API to create service meet condition
+4. Go to Service Collection manager, verify Collection infor
+5. Go to SF to verify service belong to this collection.</t>
+  </si>
+  <si>
+    <t>The service meet condition should be shown in collection</t>
+  </si>
+  <si>
+    <t>SC18</t>
+  </si>
+  <si>
+    <t>Verify automated collection when service belong collection does not meet the condition</t>
+  </si>
+  <si>
+    <t>1. Login to Dashboard
+2. Go to 2. Go to Services &gt;&gt; Create service collection (Automated)
+3. Call API to create service meet condition
+4. Go to Service Collection manager, verify Collection infor
+5. Update service to service not meet condition.
+6. Go to Service Collection manager, verify Collection infor
+7. Go to SF to verify service belong to this collection.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -364,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -380,6 +424,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,18 +711,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.77734375"/>
-    <col min="2" max="2" customWidth="true" width="46.33203125"/>
-    <col min="3" max="3" customWidth="true" width="60.0"/>
-    <col min="4" max="4" customWidth="true" width="72.5546875"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60" customWidth="1"/>
+    <col min="4" max="4" width="72.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -708,10 +758,10 @@
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="F2" t="s" s="0">
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -728,7 +778,7 @@
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="3"/>
@@ -746,7 +796,7 @@
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>62</v>
       </c>
       <c r="F4" s="3"/>
@@ -764,7 +814,7 @@
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>62</v>
       </c>
       <c r="F5" s="3"/>
@@ -782,7 +832,7 @@
       <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>62</v>
       </c>
       <c r="F6" s="3"/>
@@ -800,7 +850,7 @@
       <c r="D7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>62</v>
       </c>
       <c r="F7" s="3"/>
@@ -818,10 +868,10 @@
       <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="F8" t="s" s="0">
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" t="s">
         <v>61</v>
       </c>
     </row>
@@ -838,7 +888,7 @@
       <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>62</v>
       </c>
       <c r="F9" s="3"/>
@@ -856,7 +906,7 @@
       <c r="D10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>62</v>
       </c>
       <c r="F10" s="3"/>
@@ -874,7 +924,7 @@
       <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>62</v>
       </c>
       <c r="F11" s="3"/>
@@ -892,7 +942,7 @@
       <c r="D12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E12" t="s" s="0">
+      <c r="E12" t="s">
         <v>62</v>
       </c>
       <c r="F12" s="3"/>
@@ -910,7 +960,7 @@
       <c r="D13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s" s="0">
+      <c r="E13" t="s">
         <v>62</v>
       </c>
       <c r="F13" s="3"/>
@@ -928,7 +978,7 @@
       <c r="D14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E14" t="s" s="0">
+      <c r="E14" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="3"/>
@@ -946,7 +996,7 @@
       <c r="D15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E15" t="s" s="0">
+      <c r="E15" t="s">
         <v>62</v>
       </c>
       <c r="F15" s="3"/>
@@ -964,10 +1014,50 @@
       <c r="D16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E16" t="s" s="0">
+      <c r="E16" t="s">
         <v>62</v>
       </c>
       <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>